<commit_message>
debug started, have done some fixes
</commit_message>
<xml_diff>
--- a/DB/insert_value_to_table.xlsx
+++ b/DB/insert_value_to_table.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Documents\PERSONAL\expert_rest_system\DB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\personal\expert_system_where_to_rest\DB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7932DCF4-C790-42B2-AA30-B2242A044DF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D133FC36-FD87-4240-B0B5-06C730453CFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="3030" windowWidth="21600" windowHeight="11385" xr2:uid="{6213EA01-1638-448B-9668-F777558A2300}"/>
+    <workbookView xWindow="675" yWindow="1335" windowWidth="17250" windowHeight="12885" xr2:uid="{6213EA01-1638-448B-9668-F777558A2300}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>profession</t>
   </si>
@@ -125,40 +125,43 @@
     <t>p14(x/now)</t>
   </si>
   <si>
-    <t>Фермер</t>
-  </si>
-  <si>
-    <t>Биолог</t>
-  </si>
-  <si>
-    <t>Сборщик на линии производства</t>
-  </si>
-  <si>
-    <t>Специалист по ремонту</t>
-  </si>
-  <si>
-    <t>Разработчик</t>
-  </si>
-  <si>
-    <t>Архитектор</t>
-  </si>
-  <si>
-    <t>Писатель</t>
-  </si>
-  <si>
-    <t>Реставратор</t>
-  </si>
-  <si>
-    <t>Менеджер торгового зала</t>
-  </si>
-  <si>
-    <t>Адвокат</t>
-  </si>
-  <si>
     <t>p3(x/now)</t>
   </si>
   <si>
     <t>p4(x/w)</t>
+  </si>
+  <si>
+    <t>label</t>
+  </si>
+  <si>
+    <t>Farmer</t>
+  </si>
+  <si>
+    <t>Biologist</t>
+  </si>
+  <si>
+    <t>Assembler on the production line</t>
+  </si>
+  <si>
+    <t>Repair Specialist</t>
+  </si>
+  <si>
+    <t>Developer</t>
+  </si>
+  <si>
+    <t>Architect</t>
+  </si>
+  <si>
+    <t>Writer</t>
+  </si>
+  <si>
+    <t>Restorer</t>
+  </si>
+  <si>
+    <t>Sales floor manager</t>
+  </si>
+  <si>
+    <t>Advocate</t>
   </si>
 </sst>
 </file>
@@ -195,12 +198,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -216,9 +220,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -256,7 +260,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -362,7 +366,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -512,10 +516,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D72E9FE-4328-4665-A636-3F6987A3AA24}">
-  <dimension ref="A1:AF12"/>
+  <dimension ref="A1:AG12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
-      <selection activeCell="X11" sqref="X11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -547,7 +551,7 @@
     <col min="48" max="48" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -570,10 +574,10 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="I1" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="J1" t="s">
         <v>7</v>
@@ -644,10 +648,13 @@
       <c r="AF1" t="s">
         <v>27</v>
       </c>
+      <c r="AG1" t="s">
+        <v>32</v>
+      </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>30</v>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="B2" s="1">
         <v>0.01</v>
@@ -719,9 +726,9 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>31</v>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="B3" s="1">
         <v>0.1</v>
@@ -793,9 +800,9 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>32</v>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="B4" s="1">
         <v>0.03</v>
@@ -867,9 +874,9 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>33</v>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="B5" s="1">
         <v>0.1</v>
@@ -941,9 +948,9 @@
         <v>7.4999999999999997E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>34</v>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="B6" s="1">
         <v>0.15</v>
@@ -1015,9 +1022,9 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>35</v>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="B7" s="1">
         <v>0.08</v>
@@ -1089,9 +1096,9 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>36</v>
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="B8" s="1">
         <v>0.05</v>
@@ -1157,9 +1164,9 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>37</v>
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>40</v>
       </c>
       <c r="B9" s="1">
         <v>0.06</v>
@@ -1231,9 +1238,9 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>38</v>
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>41</v>
       </c>
       <c r="B10" s="1">
         <v>0.09</v>
@@ -1305,9 +1312,9 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>39</v>
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="B11" s="1">
         <v>0.1</v>
@@ -1379,7 +1386,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
     </row>
   </sheetData>

</xml_diff>